<commit_message>
Add JSON export and configurable header/data rows
Introduces JSON export functionality and allows configuration of header and first data row indices via YAML. Updates split-column operation to support new headers, improves CSV export to respect header/data row settings, and updates documentation and examples accordingly. Also bumps version to 0.1.2.
</commit_message>
<xml_diff>
--- a/example/result.xlsx
+++ b/example/result.xlsx
@@ -14,15 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="23">
-  <si>
-    <t>No.</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="13">
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Product-Code</t>
+  </si>
+  <si>
+    <t>Product-Name</t>
   </si>
   <si>
     <t>VG-WHITE</t>
@@ -43,46 +43,16 @@
     <t>B Necklace</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>VG</t>
-  </si>
-  <si>
-    <t>WHITE</t>
-  </si>
-  <si>
-    <t>GH</t>
-  </si>
-  <si>
-    <t>BLUE</t>
-  </si>
-  <si>
-    <t>BN</t>
-  </si>
-  <si>
-    <t>PURPLE</t>
-  </si>
-  <si>
-    <t>NAME</t>
-  </si>
-  <si>
-    <t>V SHIRT</t>
-  </si>
-  <si>
-    <t>G HANDBAG</t>
-  </si>
-  <si>
-    <t>B NECKLACE</t>
-  </si>
-  <si>
-    <t>V - SHIRT</t>
-  </si>
-  <si>
-    <t>G - HANDBAG</t>
-  </si>
-  <si>
-    <t>B - NECKLACE</t>
+    <t>Product,Name</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>product_code</t>
+  </si>
+  <si>
+    <t>product_name</t>
   </si>
 </sst>
 </file>
@@ -1004,10 +974,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1016,24 +986,18 @@
     <col min="3" max="3" width="11.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1041,16 +1005,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1058,16 +1016,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1075,13 +1027,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>